<commit_message>
Reference Genome Assembly Test cases - 5
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_RefGenAssembly-GRCh37.xlsx
+++ b/InputFiles/TC01_CDS_Filter_RefGenAssembly-GRCh37.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation 0707\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D36361-8609-45EF-B39E-F25CBE985C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D7A5EE-698A-4544-A633-1850A2EB5CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -57,63 +57,108 @@
     <t>ParticipantsTab</t>
   </si>
   <si>
-    <t>MATCH (f:file)
-Match (f)&lt;--(g:genomic_info)
-WHERE g.reference_genome_assembly in ['GRCh37']
-MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p,f, s, collect(distinct samp.sample_id) as samp
-RETURN
-count(distinct s) AS Studies,
-count(distinct p) AS Participants,
-count(distinct samp) AS Samples,
-count(distinct f) AS Files</t>
-  </si>
-  <si>
-    <t>Match (f)&lt;--(g:genomic_info)
-WHERE g.reference_genome_assembly in ['GRCh37']
-MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p, s, collect(distinct samp.sample_id) as samp
+    <t>TC01_CDS_Filter_RefGenAssembly-GRCh37_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_CDS_Filter_RefGenAssembly-GRCh37_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (p:participant)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+WITH s, p, samp, f, g, diag
+WHERE g.reference_genome_assembly in ['GRCh37'] 
+WITH p
+OPTIONAL MATCH (p)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
 RETURN 
 coalesce(p.participant_id,'') as `Participant ID`,
 coalesce(s.study_name, '') as `Study Name`,
 coalesce(s.phs_accession,'') as `Accession`,
 coalesce(p.gender,'') as `Gender`,
 coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY `Participant ID`LIMIT 100</t>
-  </si>
-  <si>
-    <t>Match (f)&lt;--(g:genomic_info)
-WHERE  g.reference_genome_assembly in ['GRCh37']
-MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
-RETURN  
- coalesce(samp.sample_id, '') as `Sample ID`,
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
-coalesce(samp.sample_tumor_status,'') as `Tumor`,
-coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER By samp.sample_id LIMIT 100</t>
-  </si>
-  <si>
-    <t>Match (f)&lt;--(g:genomic_info)
+ORDER BY p.participant_id limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (samp:sample)--&gt;(p:participant)--&gt;(s:study)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+WITH s, p, samp, f, g, diag
 WHERE g.reference_genome_assembly in ['GRCh37']
-MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p,s,f,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
-RETURN 
-    coalesce(f.file_name, '') as `File Name`,
+WITH DISTINCT s, p, samp
+RETURN
+    coalesce(samp.sample_id, '') as `Sample ID`,
+    coalesce(p.participant_id,'') as `Participant ID`,
     coalesce(s.study_name, '') as `Study Name`,
     coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.participant_id,'') as `Participant ID`,
+    coalesce(samp.sample_tumor_status,'') as `Tumor`,
+    coalesce(samp.sample_type,'') as `Analyte Type`
+ORDER BY samp.sample_id limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)&lt;--(f)
+OPTIONAL MATCH (samp)--&gt;(p:participant)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+WITH s, p, samp, f, g, diag
+WHERE g.reference_genome_assembly in ['GRCh37']
+WITH DISTINCT f, s, p, samp
+RETURN
+    coalesce(f.file_name, '') as `File Name`,
+    coalesce(s.study_name,'') as `Study Name`,
+    coalesce(s.phs_accession,'') as `Accession`,
+    coalesce(p.participant_id, '') as `Participant ID`,
     coalesce(samp.sample_id, '') as `Sample ID`,
     coalesce(f.file_type, '') as `File Type`
-ORDER By f.file_name LIMIT 100</t>
-  </si>
-  <si>
-    <t>TC01_CDS_Filter_RefGenAssembly-GRCh37_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_CDS_Filter_RefGenAssembly-GRCh37_WebData.xlsx</t>
+ORDER BY f.file_name limit 100</t>
+  </si>
+  <si>
+    <t>CALL{
+    MATCH (p:participant)--&gt;(s:study)
+    OPTIONAL MATCH (samp:sample)--&gt;(p)
+    OPTIONAL MATCH (samp)&lt;--(f:file)
+    OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+    WITH s, p, samp, f, g, diag
+    WHERE g.reference_genome_assembly in ['GRCh37']
+    RETURN 
+        count(distinct p) AS num_participants
+}
+WITH num_participants
+CALL {
+    MATCH (samp:sample)--&gt;(p:participant)--&gt;(s)
+    OPTIONAL MATCH (samp)&lt;--(f:file)
+    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+    OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+    WITH s, p, samp, f, g, diag
+    WHERE g.reference_genome_assembly in ['GRCh37']
+    RETURN 
+        count(distinct samp) AS num_samples
+}
+WITH num_participants, num_samples
+CALL {
+    MATCH (f:file)--&gt;(s:study)
+    OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+    OPTIONAL MATCH (samp:sample)&lt;--(f)
+    OPTIONAL MATCH (p:participant)&lt;--(samp)
+    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+    WITH s, p, samp, f, g, diag
+    WHERE g.reference_genome_assembly in ['GRCh37']
+    RETURN 
+        count(distinct s) AS num_studies,
+        count(distinct f) AS num_files
+}
+RETURN 
+    num_studies AS Studies,
+    num_participants AS Participants,
+    num_samples AS Samples,
+    num_files AS `Files`</t>
   </si>
 </sst>
 </file>
@@ -493,21 +538,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -524,62 +569,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="242.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="242.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="260.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="260.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="279.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="279.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
     </row>
   </sheetData>

</xml_diff>